<commit_message>
made comparison table of t-test results of all the classifiers versus rocket
</commit_message>
<xml_diff>
--- a/Evaluation/cross_validation_accuracies.xlsx
+++ b/Evaluation/cross_validation_accuracies.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\t-test accuracy results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\ExerciseClassification\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F858BF3-B7D5-4C77-BD9B-8A0E9FA87B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7A7CB6-1DA1-4109-965F-F89D59C7E644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CV Accuracies" sheetId="1" r:id="rId1"/>
-    <sheet name="Classifiers Rankings" sheetId="2" r:id="rId2"/>
+    <sheet name="CV performance metrics" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>AdaBoost</t>
   </si>
@@ -104,13 +104,41 @@
   </si>
   <si>
     <t>Mean Accuracy</t>
+  </si>
+  <si>
+    <t>Classifier</t>
+  </si>
+  <si>
+    <t>Balanced Accuracy</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>AUROC</t>
+  </si>
+  <si>
+    <t>Train time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="175" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +157,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,13 +209,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,22 +501,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -514,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -549,7 +587,7 @@
         <v>0.985164835164835</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -584,7 +622,7 @@
         <v>0.97087912087911998</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -619,7 +657,7 @@
         <v>0.99285714285714199</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -654,7 +692,7 @@
         <v>0.85277777777777697</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -689,7 +727,7 @@
         <v>0.68055555555555503</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -724,7 +762,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -759,7 +797,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -794,7 +832,7 @@
         <v>0.84722222222222199</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -829,7 +867,7 @@
         <v>0.52222222222222203</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -864,7 +902,7 @@
         <v>0.47777777777777702</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -899,7 +937,7 @@
         <v>0.78333333333333299</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -934,7 +972,7 @@
         <v>0.94166666666666599</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -969,7 +1007,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1004,7 +1042,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -1046,582 +1084,305 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55ED89EE-7469-4F55-84FE-E6AA3CB2B27A}">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47248FE-82B7-4661-92F5-889C765EB7FE}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="7">
+        <v>0.19166666666666601</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.19312499999999999</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.15518249011707699</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.19166666666666601</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.12927039008657401</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.58086777553763402</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.88079710006713796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B3" s="7">
+        <v>0.97777777777777697</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.97562499999999996</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.98232804232804205</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.97777777777777697</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.976453022286355</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.99629116263440798</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2323.28471524715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="B4" s="7">
+        <v>0.43333333333333302</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.4325</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.471711860670193</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.43333333333333302</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.42579639496306099</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.676209677419354</v>
+      </c>
+      <c r="H4" s="6">
+        <v>8.9844751358032202E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="B5" s="7">
+        <v>0.97777777777777697</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.97624999999999995</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.98249999999999904</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.97777777777777697</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.97656164822831504</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.98724798387096702</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5.35118579864501E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="B6" s="7">
+        <v>0.85833333333333295</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.85687499999999905</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.88194775132275105</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.85833333333333295</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.85622067747067698</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.97303007392473095</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3.5009384155273402E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="B7" s="7">
+        <v>0.70555555555555505</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.70937499999999998</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.723498677248677</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.70555555555555505</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.70102954144620799</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.93178483422938996</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.81888127326965299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="B8" s="7">
+        <v>0.76111111111111096</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.76375000000000004</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.79465828924162196</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.76111111111111096</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.76161014911014902</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.93856406810035797</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2.0004034042358301E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="B9" s="7">
+        <v>0.82222222222222197</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.823124999999999</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.84460317460317402</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.82222222222222197</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.818966049382716</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.97612847222222199</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.359440422058105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="B10" s="7">
+        <v>0.99166666666666603</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.99062499999999998</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.993148148148148</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.99166666666666603</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.991478274811608</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.99521169354838701</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.23059885501861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.76153846153846105</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.79780219780219697</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.969780219780219</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.88736263736263699</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.85714285714285698</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.947252747252747</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.985164835164835</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.68351648351648298</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.86538461538461497</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.962087912087912</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.81978021978021898</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.85714285714285698</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.91813186813186798</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.97087912087911998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.68076923076923002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.88021978021977998</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.969780219780219</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.89560439560439498</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.79725274725274697</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.97032967032966999</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.99285714285714199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.17777777777777701</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.93333333333333302</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.43611111111111101</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.96666666666666601</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.82777777777777695</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.66666666666666596</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.66111111111111098</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.76111111111111096</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.98888888888888804</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.85277777777777697</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.27222222222222198</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.82222222222222197</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.39722222222222198</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.76388888888888795</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.66666666666666596</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.57777777777777695</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.54722222222222205</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.63611111111111096</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.96111111111111003</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.68055555555555503</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.94722222222222197</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.85277777777777697</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.688888888888888</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.61944444444444402</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.53611111111111098</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.98611111111111105</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.16111111111111101</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.25555555555555498</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.54722222222222205</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.50555555555555498</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.36944444444444402</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.452777777777777</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.76388888888888895</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.23611111111111099</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.95277777777777695</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.969444444444444</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.74444444444444402</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.63333333333333297</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.60833333333333295</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.78333333333333299</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0.98333333333333295</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.84722222222222199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.194444444444444</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.78611111111111098</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.280555555555555</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.69444444444444398</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.49166666666666597</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.39722222222222198</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.41388888888888797</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.52222222222222203</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.88611111111111096</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0.52222222222222203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.141666666666666</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.60277777777777697</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.15833333333333299</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.30277777777777698</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.297222222222222</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.30555555555555503</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.358333333333333</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0.47777777777777702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.241666666666666</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.91388888888888797</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.49722222222222201</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.90833333333333299</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.69444444444444398</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.62222222222222201</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.55833333333333302</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0.74444444444444402</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0.96111111111111103</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0.78333333333333299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.19166666666666601</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.97777777777777697</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.43333333333333302</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.97777777777777697</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.85833333333333295</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.70555555555555505</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.76111111111111096</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.82222222222222197</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.99166666666666603</v>
-      </c>
-      <c r="K13" s="5">
+      <c r="B11" s="7">
         <v>0.94166666666666599</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.483333333333333</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.88333333333333297</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.53888888888888897</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.80555555555555503</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.69444444444444398</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.73333333333333295</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.76666666666666605</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0.99444444444444402</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.47777777777777702</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.97777777777777697</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.594444444444444</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.98333333333333295</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.81666666666666599</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.688888888888888</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0.71111111111111103</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.49444444444444402</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.98888888888888804</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.56111111111111101</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.97777777777777697</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.82777777777777695</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0.81666666666666599</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0.87777777777777699</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0.938888888888888</v>
+      <c r="C11" s="8">
+        <v>0.94125000000000003</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.95348544973544902</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.94166666666666599</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.940586219336219</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.99330197132616405</v>
+      </c>
+      <c r="H11" s="6">
+        <v>23.204096603393499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>